<commit_message>
Update picks with latest week data
</commit_message>
<xml_diff>
--- a/nfl_picks_2025.xlsx
+++ b/nfl_picks_2025.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\fantasy python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E979C576-262F-4BBF-834E-F07F40CB496F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6A33FA9-85FE-4F10-AFB0-FEFD6431297D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="50" windowWidth="25600" windowHeight="15230" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="50" windowWidth="25600" windowHeight="15230" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1801" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1897" uniqueCount="194">
   <si>
     <t>week1</t>
   </si>
@@ -640,12 +640,24 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -675,11 +687,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5947,7 +5963,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:P27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
@@ -6627,9 +6643,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:P27"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L22" sqref="L22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="21.6328125" customWidth="1"/>
+    <col min="8" max="8" width="23.1796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.6328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.54296875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
@@ -6676,212 +6700,643 @@
       <c r="A2" t="s">
         <v>72</v>
       </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>7</v>
       </c>
-      <c r="H3" t="s">
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="3"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>73</v>
       </c>
-      <c r="H4" t="s">
+      <c r="B4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="P4" s="3"/>
+    </row>
+    <row r="5" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="H5" t="s">
+      <c r="B5" s="5"/>
+      <c r="C5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I5" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="J5" t="s">
+      <c r="J5" s="5" t="s">
         <v>76</v>
       </c>
+      <c r="K5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="5"/>
+      <c r="O5" s="5"/>
+      <c r="P5" s="5"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="H6" t="s">
+      <c r="B6" s="3"/>
+      <c r="C6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="I6" t="s">
-        <v>22</v>
-      </c>
-      <c r="J6" t="s">
+      <c r="I6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J6" s="2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="H7" t="s">
+      <c r="K6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="N6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="O6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="P6" s="3"/>
+    </row>
+    <row r="7" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="I7" t="s">
-        <v>22</v>
-      </c>
-      <c r="J7" t="s">
+      <c r="I7" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="J7" s="5" t="s">
         <v>43</v>
       </c>
+      <c r="K7" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="L7" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="M7" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="N7" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="O7" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="P7" s="5" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="H8" t="s">
+      <c r="B8" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H8" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="I8" t="s">
-        <v>22</v>
-      </c>
-      <c r="J8" t="s">
+      <c r="I8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J8" s="2" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="H9" t="s">
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="3"/>
+      <c r="P8" s="3"/>
+    </row>
+    <row r="9" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="I9" t="s">
-        <v>22</v>
-      </c>
-      <c r="J9" t="s">
+      <c r="I9" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="J9" s="5" t="s">
         <v>49</v>
       </c>
+      <c r="K9" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="L9" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="M9" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="N9" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="O9" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="P9" s="5" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="H10" t="s">
+      <c r="B10" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G10" s="3"/>
+      <c r="H10" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I10" t="s">
-        <v>22</v>
-      </c>
-      <c r="J10" t="s">
+      <c r="I10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J10" s="2" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="H11" t="s">
+      <c r="K10" s="3"/>
+      <c r="L10" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="M10" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="N10" s="3"/>
+      <c r="O10" s="3"/>
+      <c r="P10" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="I11" t="s">
-        <v>22</v>
-      </c>
-      <c r="J11" t="s">
+      <c r="I11" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="J11" s="5" t="s">
         <v>46</v>
       </c>
+      <c r="K11" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="L11" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="M11" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="N11" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="O11" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="P11" s="5" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="H12" t="s">
+      <c r="B12" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H12" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="I12" t="s">
-        <v>22</v>
-      </c>
-      <c r="J12" t="s">
+      <c r="I12" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J12" s="2" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="H13" t="s">
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="O12" s="3"/>
+      <c r="P12" s="3"/>
+    </row>
+    <row r="13" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="I13" t="s">
+      <c r="I13" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="J13" t="s">
+      <c r="J13" s="5" t="s">
         <v>47</v>
       </c>
+      <c r="K13" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="L13" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="M13" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="N13" s="5"/>
+      <c r="O13" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="P13" s="5" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="H14" t="s">
+      <c r="B14" s="3"/>
+      <c r="C14" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="I14" t="s">
+      <c r="I14" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="J14" t="s">
+      <c r="J14" s="2" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="H15" t="s">
+      <c r="K14" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3"/>
+      <c r="N14" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="O14" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="P14" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H15" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="I15" t="s">
+      <c r="I15" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="J15" t="s">
+      <c r="J15" s="5" t="s">
         <v>17</v>
       </c>
+      <c r="K15" s="5"/>
+      <c r="L15" s="5"/>
+      <c r="M15" s="5"/>
+      <c r="N15" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="O15" s="5"/>
+      <c r="P15" s="5"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="H16" t="s">
+      <c r="B16" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G16" s="3"/>
+      <c r="H16" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="I16" t="s">
+      <c r="I16" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="J16" t="s">
+      <c r="J16" s="2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="H17" t="s">
+      <c r="K16" s="3"/>
+      <c r="L16" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="M16" s="3"/>
+      <c r="N16" s="3"/>
+      <c r="O16" s="3"/>
+      <c r="P16" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B17" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H17" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="I17" t="s">
+      <c r="I17" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="J17" t="s">
+      <c r="J17" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K17" s="5"/>
+      <c r="L17" s="5"/>
+      <c r="M17" s="5"/>
+      <c r="N17" s="5"/>
+      <c r="O17" s="5"/>
+      <c r="P17" s="5"/>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>77</v>
       </c>
-      <c r="H18" t="s">
+      <c r="B18" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G18" s="3"/>
+      <c r="H18" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="I18" t="s">
+      <c r="I18" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="J18" t="s">
+      <c r="J18" s="2" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="H19" t="s">
+      <c r="K18" s="3"/>
+      <c r="L18" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="M18" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="N18" s="3"/>
+      <c r="O18" s="3"/>
+      <c r="P18" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="I19" t="s">
+      <c r="I19" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="J19" t="s">
+      <c r="J19" s="5" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K19" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="L19" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="M19" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="N19" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="O19" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="P19" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="K20">
+        <v>34</v>
+      </c>
+      <c r="L20">
+        <v>39</v>
+      </c>
+      <c r="M20">
+        <v>52</v>
+      </c>
+      <c r="N20">
+        <v>46</v>
+      </c>
+      <c r="O20">
+        <v>45</v>
+      </c>
+      <c r="P20">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B23" t="s">
         <v>1</v>
       </c>
@@ -6901,12 +7356,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>56</v>
       </c>
@@ -6929,7 +7384,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>57</v>
       </c>
@@ -6952,7 +7407,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>58</v>
       </c>

</xml_diff>

<commit_message>
Add team breakdown tab and Week 5 picks Excel file
</commit_message>
<xml_diff>
--- a/nfl_picks_2025.xlsx
+++ b/nfl_picks_2025.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\fantasy python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6A33FA9-85FE-4F10-AFB0-FEFD6431297D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EC12033-F35D-42EC-BEEA-84DA6795604D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="50" windowWidth="25600" windowHeight="15230" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="50" windowWidth="25600" windowHeight="15230" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1897" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1981" uniqueCount="194">
   <si>
     <t>week1</t>
   </si>
@@ -687,7 +687,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -696,6 +696,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6643,8 +6646,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:P27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7172,10 +7175,10 @@
       <c r="B16" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="E16" s="3" t="s">
         <v>15</v>
       </c>
@@ -7439,9 +7442,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:P27"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="8" max="8" width="23.1796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.6328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.90625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
@@ -7516,11 +7526,44 @@
       <c r="J4" t="s">
         <v>47</v>
       </c>
+      <c r="K4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L4" t="s">
+        <v>15</v>
+      </c>
+      <c r="M4" t="s">
+        <v>15</v>
+      </c>
+      <c r="N4" t="s">
+        <v>15</v>
+      </c>
+      <c r="O4" t="s">
+        <v>15</v>
+      </c>
+      <c r="P4" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>83</v>
       </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" t="s">
+        <v>15</v>
+      </c>
       <c r="H5" t="s">
         <v>51</v>
       </c>
@@ -7530,8 +7573,26 @@
       <c r="J5" t="s">
         <v>84</v>
       </c>
+      <c r="P5" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" t="s">
+        <v>15</v>
+      </c>
       <c r="H6" t="s">
         <v>12</v>
       </c>
@@ -7540,6 +7601,9 @@
       </c>
       <c r="J6" t="s">
         <v>35</v>
+      </c>
+      <c r="N6" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.35">
@@ -7552,8 +7616,41 @@
       <c r="J7" t="s">
         <v>14</v>
       </c>
+      <c r="K7" t="s">
+        <v>15</v>
+      </c>
+      <c r="L7" t="s">
+        <v>15</v>
+      </c>
+      <c r="M7" t="s">
+        <v>15</v>
+      </c>
+      <c r="N7" t="s">
+        <v>15</v>
+      </c>
+      <c r="O7" t="s">
+        <v>15</v>
+      </c>
+      <c r="P7" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" t="s">
+        <v>15</v>
+      </c>
       <c r="H8" t="s">
         <v>46</v>
       </c>
@@ -7562,6 +7659,9 @@
       </c>
       <c r="J8" t="s">
         <v>48</v>
+      </c>
+      <c r="L8" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.35">
@@ -7574,8 +7674,35 @@
       <c r="J9" t="s">
         <v>31</v>
       </c>
+      <c r="K9" t="s">
+        <v>15</v>
+      </c>
+      <c r="L9" t="s">
+        <v>15</v>
+      </c>
+      <c r="M9" t="s">
+        <v>15</v>
+      </c>
+      <c r="N9" t="s">
+        <v>15</v>
+      </c>
+      <c r="O9" t="s">
+        <v>15</v>
+      </c>
+      <c r="P9" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="B10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" t="s">
+        <v>15</v>
+      </c>
       <c r="H10" t="s">
         <v>30</v>
       </c>
@@ -7585,8 +7712,32 @@
       <c r="J10" t="s">
         <v>24</v>
       </c>
+      <c r="L10" t="s">
+        <v>15</v>
+      </c>
+      <c r="M10" t="s">
+        <v>15</v>
+      </c>
+      <c r="P10" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="C11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F11" t="s">
+        <v>15</v>
+      </c>
+      <c r="G11" t="s">
+        <v>15</v>
+      </c>
       <c r="H11" t="s">
         <v>32</v>
       </c>
@@ -7596,8 +7747,20 @@
       <c r="J11" t="s">
         <v>23</v>
       </c>
+      <c r="K11" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="C12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" t="s">
+        <v>15</v>
+      </c>
+      <c r="G12" t="s">
+        <v>15</v>
+      </c>
       <c r="H12" t="s">
         <v>36</v>
       </c>
@@ -7606,6 +7769,15 @@
       </c>
       <c r="J12" t="s">
         <v>40</v>
+      </c>
+      <c r="K12" t="s">
+        <v>15</v>
+      </c>
+      <c r="N12" t="s">
+        <v>15</v>
+      </c>
+      <c r="O12" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.35">
@@ -7618,8 +7790,44 @@
       <c r="J13" t="s">
         <v>21</v>
       </c>
+      <c r="K13" t="s">
+        <v>15</v>
+      </c>
+      <c r="L13" t="s">
+        <v>15</v>
+      </c>
+      <c r="M13" t="s">
+        <v>15</v>
+      </c>
+      <c r="N13" t="s">
+        <v>15</v>
+      </c>
+      <c r="O13" t="s">
+        <v>15</v>
+      </c>
+      <c r="P13" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="B14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" t="s">
+        <v>15</v>
+      </c>
+      <c r="F14" t="s">
+        <v>15</v>
+      </c>
+      <c r="G14" t="s">
+        <v>15</v>
+      </c>
       <c r="H14" t="s">
         <v>43</v>
       </c>
@@ -7631,6 +7839,15 @@
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="C15" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" t="s">
+        <v>15</v>
+      </c>
+      <c r="G15" t="s">
+        <v>15</v>
+      </c>
       <c r="H15" t="s">
         <v>33</v>
       </c>
@@ -7639,6 +7856,15 @@
       </c>
       <c r="J15" t="s">
         <v>64</v>
+      </c>
+      <c r="K15" t="s">
+        <v>15</v>
+      </c>
+      <c r="N15" t="s">
+        <v>15</v>
+      </c>
+      <c r="O15" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.35">
@@ -7651,11 +7877,41 @@
       <c r="J16" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K16" t="s">
+        <v>15</v>
+      </c>
+      <c r="L16" t="s">
+        <v>15</v>
+      </c>
+      <c r="M16" t="s">
+        <v>15</v>
+      </c>
+      <c r="N16" t="s">
+        <v>15</v>
+      </c>
+      <c r="O16" t="s">
+        <v>15</v>
+      </c>
+      <c r="P16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>85</v>
       </c>
+      <c r="B17" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" t="s">
+        <v>15</v>
+      </c>
+      <c r="E17" t="s">
+        <v>15</v>
+      </c>
+      <c r="F17" t="s">
+        <v>15</v>
+      </c>
       <c r="H17" t="s">
         <v>17</v>
       </c>
@@ -7665,18 +7921,44 @@
       <c r="J17" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="L17" t="s">
+        <v>15</v>
+      </c>
+      <c r="P17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="B18">
+        <v>49</v>
+      </c>
+      <c r="D18">
+        <v>44</v>
+      </c>
+      <c r="E18">
+        <v>48</v>
+      </c>
+      <c r="F18">
+        <v>46</v>
+      </c>
+      <c r="L18">
+        <v>39</v>
+      </c>
+      <c r="P18">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B23" t="s">
         <v>1</v>
       </c>
@@ -7696,12 +7978,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>56</v>
       </c>
@@ -7724,7 +8006,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>57</v>
       </c>
@@ -7747,7 +8029,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>58</v>
       </c>

</xml_diff>